<commit_message>
made proper folder structure
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Final_450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EFFA4B2-C94B-40B6-9488-BCE49438FFFD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{197A22E8-6E6E-4661-9670-13288231994F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
+    <workbookView xWindow="9620" yWindow="50" windowWidth="9530" windowHeight="10100" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1892,8 +1892,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="94" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="56" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="21"/>
@@ -2061,7 +2061,7 @@
       <c r="B18" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="9">
+      <c r="C18" s="12">
         <v>13</v>
       </c>
     </row>

</xml_diff>